<commit_message>
updating to work with VS2015
</commit_message>
<xml_diff>
--- a/Excel OData Connector/Excel OData Connector/ODSampleData/bin/Debug/Book1.xlsx
+++ b/Excel OData Connector/Excel OData Connector/ODSampleData/bin/Debug/Book1.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R8ae54cd93abd42d4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R022328e964a74cd0"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R97937e6f2e894e4d"/>
+  <wetp:taskpane dockstate="" visibility="1" width="700" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5a91471a06a645a9"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1eabe65a-0ac5-4132-bd22-27e7e806f3de}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c23dfeea-7e89-496f-ae0f-0cedd7d4f9a9}">
   <we:reference id="e57a32a9-958a-4579-809f-df1a11a64752" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
add button on Data tab using add-in commands
</commit_message>
<xml_diff>
--- a/Excel OData Connector/Excel OData Connector/ODSampleData/bin/Debug/Book1.xlsx
+++ b/Excel OData Connector/Excel OData Connector/ODSampleData/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R022328e964a74cd0"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R65a98bf3b7c04397"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,14 +10,14 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="700" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5a91471a06a645a9"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R600faae9e0384aaa"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c23dfeea-7e89-496f-ae0f-0cedd7d4f9a9}">
-  <we:reference id="e57a32a9-958a-4579-809f-df1a11a64752" version="1.0.0.0" store="developer" storeType="Registry"/>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b4015073-2c98-4e00-b5e9-eeccfd6a2bd9}">
+  <we:reference id="e57a32a9-958a-4579-809f-df1a11a64751" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>
   <we:bindings/>

</xml_diff>